<commit_message>
shop management & using unittest
</commit_message>
<xml_diff>
--- a/Admin.xlsx
+++ b/Admin.xlsx
@@ -5,11 +5,11 @@
   <workbookPr filterPrivacy="1" checkCompatibility="1" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yudu/Google Drive/iKnow/test/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yudu/Google Drive/iKnowTesting/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000"/>
+    <workbookView minimized="1" xWindow="14440" yWindow="460" windowWidth="14360" windowHeight="17540"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="7" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="48">
   <si>
     <t>【通过/不通过/其他……】</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -157,7 +157,22 @@
     <t>Shop</t>
   </si>
   <si>
-    <t>Click 商家-查询, choose one shop, click 查询,</t>
+    <t>Main Framework</t>
+  </si>
+  <si>
+    <t>click main title located at left top return to welcome page</t>
+  </si>
+  <si>
+    <t>Click 管理信息-商家-查询, 进入选择商家页面。</t>
+  </si>
+  <si>
+    <t>在商家选择页面中的下拉菜单中选择商家，click查询，显示商家信息</t>
+  </si>
+  <si>
+    <t>click 编辑，更改商家信息后，点击保存，商户信息更改到数据库。</t>
+  </si>
+  <si>
+    <t>点击删除后，提示确认删除信息，点击ok，删除商户信息</t>
   </si>
 </sst>
 </file>
@@ -778,6 +793,21 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -819,21 +849,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="118">
@@ -1266,11 +1281,11 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:H71"/>
+  <dimension ref="A1:H77"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
+      <selection pane="bottomLeft" activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1313,7 +1328,7 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="28">
+      <c r="A2" s="14">
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
@@ -1326,780 +1341,854 @@
       <c r="G2" s="6"/>
       <c r="H2" s="7"/>
     </row>
-    <row r="3" spans="1:8" s="30" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="29"/>
-      <c r="B3" s="29">
+    <row r="3" spans="1:8" s="16" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="15"/>
+      <c r="B3" s="15">
         <v>1.1000000000000001</v>
       </c>
-      <c r="C3" s="29" t="s">
+      <c r="C3" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-    </row>
-    <row r="4" spans="1:8" s="30" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="29"/>
-      <c r="B4" s="29">
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+    </row>
+    <row r="4" spans="1:8" s="16" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="15"/>
+      <c r="B4" s="15">
         <v>1.2</v>
       </c>
-      <c r="C4" s="29" t="s">
+      <c r="C4" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="29"/>
-      <c r="G4" s="29"/>
-      <c r="H4" s="29"/>
-    </row>
-    <row r="5" spans="1:8" s="30" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="29"/>
-      <c r="B5" s="29">
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+    </row>
+    <row r="5" spans="1:8" s="16" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="15"/>
+      <c r="B5" s="15">
         <v>1.3</v>
       </c>
-      <c r="C5" s="29" t="s">
+      <c r="C5" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="29"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="29"/>
-      <c r="H5" s="29"/>
-    </row>
-    <row r="6" spans="1:8" s="30" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="29"/>
-      <c r="B6" s="29">
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+    </row>
+    <row r="6" spans="1:8" s="16" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="15"/>
+      <c r="B6" s="15">
         <v>1.4</v>
       </c>
-      <c r="C6" s="29" t="s">
+      <c r="C6" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="29"/>
-      <c r="E6" s="29"/>
-      <c r="F6" s="29"/>
-      <c r="G6" s="29"/>
-      <c r="H6" s="29"/>
-    </row>
-    <row r="7" spans="1:8" s="32" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="31"/>
-      <c r="B7" s="29">
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+    </row>
+    <row r="7" spans="1:8" s="18" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="17"/>
+      <c r="B7" s="15">
         <v>1.5</v>
       </c>
-      <c r="C7" s="31" t="s">
+      <c r="C7" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="31"/>
-      <c r="E7" s="31"/>
-      <c r="F7" s="31"/>
-      <c r="G7" s="31"/>
-      <c r="H7" s="31"/>
-    </row>
-    <row r="8" spans="1:8" s="30" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="29"/>
-      <c r="B8" s="29"/>
-      <c r="C8" s="29"/>
-      <c r="D8" s="29"/>
-      <c r="E8" s="29"/>
-      <c r="F8" s="29"/>
-      <c r="G8" s="29"/>
-      <c r="H8" s="29"/>
-    </row>
-    <row r="9" spans="1:8" s="30" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A9" s="29"/>
-      <c r="B9" s="29" t="s">
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="17"/>
+    </row>
+    <row r="8" spans="1:8" s="16" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="15">
+        <v>2</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+    </row>
+    <row r="9" spans="1:8" s="16" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="15"/>
+      <c r="B9" s="15">
+        <v>2.1</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+    </row>
+    <row r="10" spans="1:8" s="16" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="15"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+    </row>
+    <row r="11" spans="1:8" s="16" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" s="15"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+    </row>
+    <row r="12" spans="1:8" s="16" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" s="15"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+    </row>
+    <row r="13" spans="1:8" s="16" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" s="15"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+    </row>
+    <row r="14" spans="1:8" s="16" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" s="15"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+    </row>
+    <row r="15" spans="1:8" s="16" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" s="15"/>
+      <c r="B15" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="29"/>
-      <c r="D9" s="29"/>
-      <c r="E9" s="29"/>
-      <c r="F9" s="29"/>
-      <c r="G9" s="29"/>
-      <c r="H9" s="29"/>
-    </row>
-    <row r="10" spans="1:8" s="30" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="29"/>
-      <c r="B10" s="29"/>
-      <c r="C10" s="29" t="s">
-        <v>42</v>
-      </c>
-      <c r="D10" s="29"/>
-      <c r="E10" s="29"/>
-      <c r="F10" s="29"/>
-      <c r="G10" s="29"/>
-      <c r="H10" s="29"/>
-    </row>
-    <row r="11" spans="1:8" s="30" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="29"/>
-      <c r="B11" s="29"/>
-      <c r="C11" s="29"/>
-      <c r="D11" s="29"/>
-      <c r="E11" s="29"/>
-      <c r="F11" s="29"/>
-      <c r="G11" s="29"/>
-      <c r="H11" s="29"/>
-    </row>
-    <row r="12" spans="1:8" s="30" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" s="29"/>
-      <c r="B12" s="29"/>
-      <c r="C12" s="29"/>
-      <c r="D12" s="29"/>
-      <c r="E12" s="29"/>
-      <c r="F12" s="29"/>
-      <c r="G12" s="29"/>
-      <c r="H12" s="29"/>
-    </row>
-    <row r="13" spans="1:8" s="30" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13" s="29"/>
-      <c r="B13" s="29"/>
-      <c r="C13" s="29"/>
-      <c r="D13" s="29"/>
-      <c r="E13" s="29"/>
-      <c r="F13" s="29"/>
-      <c r="G13" s="29"/>
-      <c r="H13" s="29"/>
-    </row>
-    <row r="14" spans="1:8" s="30" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="29"/>
-      <c r="B14" s="29"/>
-      <c r="C14" s="29"/>
-      <c r="D14" s="29"/>
-      <c r="E14" s="29"/>
-      <c r="F14" s="29"/>
-      <c r="G14" s="29"/>
-      <c r="H14" s="29"/>
-    </row>
-    <row r="15" spans="1:8" s="30" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A15" s="29"/>
-      <c r="B15" s="29"/>
-      <c r="C15" s="29"/>
-      <c r="D15" s="29"/>
-      <c r="E15" s="29"/>
-      <c r="F15" s="29"/>
-      <c r="G15" s="29"/>
-      <c r="H15" s="29"/>
-    </row>
-    <row r="16" spans="1:8" s="30" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A16" s="29"/>
-      <c r="B16" s="29"/>
-      <c r="C16" s="29"/>
-      <c r="D16" s="29"/>
-      <c r="E16" s="29"/>
-      <c r="F16" s="29"/>
-      <c r="G16" s="29"/>
-      <c r="H16" s="29"/>
-    </row>
-    <row r="17" spans="1:8" s="30" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A17" s="29"/>
-      <c r="B17" s="29"/>
-      <c r="C17" s="29"/>
-      <c r="D17" s="29"/>
-      <c r="E17" s="29"/>
-      <c r="F17" s="29"/>
-      <c r="G17" s="29"/>
-      <c r="H17" s="29"/>
-    </row>
-    <row r="18" spans="1:8" s="30" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A18" s="29"/>
-      <c r="B18" s="29"/>
-      <c r="C18" s="29"/>
-      <c r="D18" s="29"/>
-      <c r="E18" s="29"/>
-      <c r="F18" s="29"/>
-      <c r="G18" s="29"/>
-      <c r="H18" s="29"/>
-    </row>
-    <row r="19" spans="1:8" s="30" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A19" s="29"/>
-      <c r="B19" s="29"/>
-      <c r="C19" s="29"/>
-      <c r="D19" s="29"/>
-      <c r="E19" s="29"/>
-      <c r="F19" s="29"/>
-      <c r="G19" s="29"/>
-      <c r="H19" s="29"/>
-    </row>
-    <row r="20" spans="1:8" s="30" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A20" s="29"/>
-      <c r="B20" s="29"/>
-      <c r="C20" s="29"/>
-      <c r="D20" s="29"/>
-      <c r="E20" s="29"/>
-      <c r="F20" s="29"/>
-      <c r="G20" s="29"/>
-      <c r="H20" s="29"/>
-    </row>
-    <row r="21" spans="1:8" s="30" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A21" s="29"/>
-      <c r="B21" s="29"/>
-      <c r="C21" s="29"/>
-      <c r="D21" s="29"/>
-      <c r="E21" s="29"/>
-      <c r="F21" s="29"/>
-      <c r="G21" s="29"/>
-      <c r="H21" s="29"/>
-    </row>
-    <row r="22" spans="1:8" s="30" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A22" s="29"/>
-      <c r="B22" s="29"/>
-      <c r="C22" s="29"/>
-      <c r="D22" s="29"/>
-      <c r="E22" s="29"/>
-      <c r="F22" s="29"/>
-      <c r="G22" s="29"/>
-      <c r="H22" s="29"/>
-    </row>
-    <row r="23" spans="1:8" s="30" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A23" s="29"/>
-      <c r="B23" s="29"/>
-      <c r="C23" s="29"/>
-      <c r="D23" s="29"/>
-      <c r="E23" s="29"/>
-      <c r="F23" s="29"/>
-      <c r="G23" s="29"/>
-      <c r="H23" s="29"/>
-    </row>
-    <row r="24" spans="1:8" s="30" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A24" s="29"/>
-      <c r="B24" s="29"/>
-      <c r="C24" s="29"/>
-      <c r="D24" s="29"/>
-      <c r="E24" s="29"/>
-      <c r="F24" s="29"/>
-      <c r="G24" s="29"/>
-      <c r="H24" s="29"/>
-    </row>
-    <row r="25" spans="1:8" s="30" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A25" s="29"/>
-      <c r="B25" s="29"/>
-      <c r="C25" s="29"/>
-      <c r="D25" s="29"/>
-      <c r="E25" s="29"/>
-      <c r="F25" s="29"/>
-      <c r="G25" s="29"/>
-      <c r="H25" s="29"/>
-    </row>
-    <row r="26" spans="1:8" s="30" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A26" s="29"/>
-      <c r="B26" s="29"/>
-      <c r="C26" s="29"/>
-      <c r="D26" s="29"/>
-      <c r="E26" s="29"/>
-      <c r="F26" s="29"/>
-      <c r="G26" s="29"/>
-      <c r="H26" s="29"/>
-    </row>
-    <row r="27" spans="1:8" s="30" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A27" s="29"/>
-      <c r="B27" s="29"/>
-      <c r="C27" s="29"/>
-      <c r="D27" s="29"/>
-      <c r="E27" s="29"/>
-      <c r="F27" s="29"/>
-      <c r="G27" s="29"/>
-      <c r="H27" s="29"/>
-    </row>
-    <row r="28" spans="1:8" s="30" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A28" s="29"/>
-      <c r="B28" s="29"/>
-      <c r="C28" s="29"/>
-      <c r="D28" s="29"/>
-      <c r="E28" s="29"/>
-      <c r="F28" s="29"/>
-      <c r="G28" s="29"/>
-      <c r="H28" s="29"/>
-    </row>
-    <row r="29" spans="1:8" s="30" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A29" s="29"/>
-      <c r="B29" s="29"/>
-      <c r="C29" s="29"/>
-      <c r="D29" s="29"/>
-      <c r="E29" s="29"/>
-      <c r="F29" s="29"/>
-      <c r="G29" s="29"/>
-      <c r="H29" s="29"/>
-    </row>
-    <row r="30" spans="1:8" s="30" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A30" s="29"/>
-      <c r="B30" s="29"/>
-      <c r="C30" s="29"/>
-      <c r="D30" s="29"/>
-      <c r="E30" s="29"/>
-      <c r="F30" s="29"/>
-      <c r="G30" s="29"/>
-      <c r="H30" s="29"/>
-    </row>
-    <row r="31" spans="1:8" s="30" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A31" s="29"/>
-      <c r="B31" s="29"/>
-      <c r="C31" s="29"/>
-      <c r="D31" s="29"/>
-      <c r="E31" s="29"/>
-      <c r="F31" s="29"/>
-      <c r="G31" s="29"/>
-      <c r="H31" s="29"/>
-    </row>
-    <row r="32" spans="1:8" s="30" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A32" s="29"/>
-      <c r="B32" s="29"/>
-      <c r="C32" s="29"/>
-      <c r="D32" s="29"/>
-      <c r="E32" s="29"/>
-      <c r="F32" s="29"/>
-      <c r="G32" s="29"/>
-      <c r="H32" s="29"/>
-    </row>
-    <row r="33" spans="1:8" s="30" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A33" s="29"/>
-      <c r="B33" s="29"/>
-      <c r="C33" s="29"/>
-      <c r="D33" s="29"/>
-      <c r="E33" s="29"/>
-      <c r="F33" s="29"/>
-      <c r="G33" s="29"/>
-      <c r="H33" s="29"/>
-    </row>
-    <row r="34" spans="1:8" s="30" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A34" s="29"/>
-      <c r="B34" s="29"/>
-      <c r="C34" s="29"/>
-      <c r="D34" s="29"/>
-      <c r="E34" s="29"/>
-      <c r="F34" s="29"/>
-      <c r="G34" s="29"/>
-      <c r="H34" s="29"/>
-    </row>
-    <row r="35" spans="1:8" s="30" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A35" s="29"/>
-      <c r="B35" s="29"/>
-      <c r="C35" s="29"/>
-      <c r="D35" s="29"/>
-      <c r="E35" s="29"/>
-      <c r="F35" s="29"/>
-      <c r="G35" s="29"/>
-      <c r="H35" s="29"/>
-    </row>
-    <row r="36" spans="1:8" s="30" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A36" s="29"/>
-      <c r="B36" s="29"/>
-      <c r="C36" s="29"/>
-      <c r="D36" s="29"/>
-      <c r="E36" s="29"/>
-      <c r="F36" s="29"/>
-      <c r="G36" s="29"/>
-      <c r="H36" s="29"/>
-    </row>
-    <row r="37" spans="1:8" s="30" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A37" s="29"/>
-      <c r="B37" s="29"/>
-      <c r="C37" s="29"/>
-      <c r="D37" s="29"/>
-      <c r="E37" s="29"/>
-      <c r="F37" s="29"/>
-      <c r="G37" s="29"/>
-      <c r="H37" s="29"/>
-    </row>
-    <row r="38" spans="1:8" s="30" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A38" s="29"/>
-      <c r="B38" s="29"/>
-      <c r="C38" s="29"/>
-      <c r="D38" s="29"/>
-      <c r="E38" s="29"/>
-      <c r="F38" s="29"/>
-      <c r="G38" s="29"/>
-      <c r="H38" s="29"/>
-    </row>
-    <row r="39" spans="1:8" s="30" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A39" s="29"/>
-      <c r="B39" s="29"/>
-      <c r="C39" s="29"/>
-      <c r="D39" s="29"/>
-      <c r="E39" s="29"/>
-      <c r="F39" s="29"/>
-      <c r="G39" s="29"/>
-      <c r="H39" s="29"/>
-    </row>
-    <row r="40" spans="1:8" s="30" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A40" s="29"/>
-      <c r="B40" s="29"/>
-      <c r="C40" s="29"/>
-      <c r="D40" s="29"/>
-      <c r="E40" s="29"/>
-      <c r="F40" s="29"/>
-      <c r="G40" s="29"/>
-      <c r="H40" s="29"/>
-    </row>
-    <row r="41" spans="1:8" s="30" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A41" s="29"/>
-      <c r="B41" s="29"/>
-      <c r="C41" s="29"/>
-      <c r="D41" s="29"/>
-      <c r="E41" s="29"/>
-      <c r="F41" s="29"/>
-      <c r="G41" s="29"/>
-      <c r="H41" s="29"/>
-    </row>
-    <row r="42" spans="1:8" s="30" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A42" s="29"/>
-      <c r="B42" s="29"/>
-      <c r="C42" s="29"/>
-      <c r="D42" s="29"/>
-      <c r="E42" s="29"/>
-      <c r="F42" s="29"/>
-      <c r="G42" s="29"/>
-      <c r="H42" s="29"/>
-    </row>
-    <row r="43" spans="1:8" s="30" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A43" s="29"/>
-      <c r="B43" s="29"/>
-      <c r="C43" s="29"/>
-      <c r="D43" s="29"/>
-      <c r="E43" s="29"/>
-      <c r="F43" s="29"/>
-      <c r="G43" s="29"/>
-      <c r="H43" s="29"/>
-    </row>
-    <row r="44" spans="1:8" s="30" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A44" s="29"/>
-      <c r="B44" s="29"/>
-      <c r="C44" s="29"/>
-      <c r="D44" s="29"/>
-      <c r="E44" s="29"/>
-      <c r="F44" s="29"/>
-      <c r="G44" s="29"/>
-      <c r="H44" s="29"/>
-    </row>
-    <row r="45" spans="1:8" s="30" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A45" s="29"/>
-      <c r="B45" s="29"/>
-      <c r="C45" s="29"/>
-      <c r="D45" s="29"/>
-      <c r="E45" s="29"/>
-      <c r="F45" s="29"/>
-      <c r="G45" s="29"/>
-      <c r="H45" s="29"/>
-    </row>
-    <row r="46" spans="1:8" s="30" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A46" s="29"/>
-      <c r="B46" s="29"/>
-      <c r="C46" s="29"/>
-      <c r="D46" s="29"/>
-      <c r="E46" s="29"/>
-      <c r="F46" s="29"/>
-      <c r="G46" s="29"/>
-      <c r="H46" s="29"/>
-    </row>
-    <row r="47" spans="1:8" s="30" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A47" s="29"/>
-      <c r="B47" s="29"/>
-      <c r="C47" s="29"/>
-      <c r="D47" s="29"/>
-      <c r="E47" s="29"/>
-      <c r="F47" s="29"/>
-      <c r="G47" s="29"/>
-      <c r="H47" s="29"/>
-    </row>
-    <row r="48" spans="1:8" s="30" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A48" s="29"/>
-      <c r="B48" s="29"/>
-      <c r="C48" s="29"/>
-      <c r="D48" s="29"/>
-      <c r="E48" s="29"/>
-      <c r="F48" s="29"/>
-      <c r="G48" s="29"/>
-      <c r="H48" s="29"/>
-    </row>
-    <row r="49" spans="1:8" s="30" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A49" s="29"/>
-      <c r="B49" s="29"/>
-      <c r="C49" s="29"/>
-      <c r="D49" s="29"/>
-      <c r="E49" s="29"/>
-      <c r="F49" s="29"/>
-      <c r="G49" s="29"/>
-      <c r="H49" s="29"/>
-    </row>
-    <row r="50" spans="1:8" s="30" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A50" s="29"/>
-      <c r="B50" s="29"/>
-      <c r="C50" s="29"/>
-      <c r="D50" s="29"/>
-      <c r="E50" s="29"/>
-      <c r="F50" s="29"/>
-      <c r="G50" s="29"/>
-      <c r="H50" s="29"/>
-    </row>
-    <row r="51" spans="1:8" s="30" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A51" s="29"/>
-      <c r="B51" s="29"/>
-      <c r="C51" s="29"/>
-      <c r="D51" s="29"/>
-      <c r="E51" s="29"/>
-      <c r="F51" s="29"/>
-      <c r="G51" s="29"/>
-      <c r="H51" s="29"/>
-    </row>
-    <row r="52" spans="1:8" s="30" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A52" s="29"/>
-      <c r="B52" s="29"/>
-      <c r="C52" s="29"/>
-      <c r="D52" s="29"/>
-      <c r="E52" s="29"/>
-      <c r="F52" s="29"/>
-      <c r="G52" s="29"/>
-      <c r="H52" s="29"/>
-    </row>
-    <row r="53" spans="1:8" s="30" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A53" s="29"/>
-      <c r="B53" s="29"/>
-      <c r="C53" s="29"/>
-      <c r="D53" s="29"/>
-      <c r="E53" s="29"/>
-      <c r="F53" s="29"/>
-      <c r="G53" s="29"/>
-      <c r="H53" s="29"/>
-    </row>
-    <row r="54" spans="1:8" s="30" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A54" s="29"/>
-      <c r="B54" s="29"/>
-      <c r="C54" s="29"/>
-      <c r="D54" s="29"/>
-      <c r="E54" s="29"/>
-      <c r="F54" s="29"/>
-      <c r="G54" s="29"/>
-      <c r="H54" s="29"/>
-    </row>
-    <row r="55" spans="1:8" s="30" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A55" s="29"/>
-      <c r="B55" s="29"/>
-      <c r="C55" s="29"/>
-      <c r="D55" s="29"/>
-      <c r="E55" s="29"/>
-      <c r="F55" s="29"/>
-      <c r="G55" s="29"/>
-      <c r="H55" s="29"/>
-    </row>
-    <row r="56" spans="1:8" s="30" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A56" s="29"/>
-      <c r="B56" s="29"/>
-      <c r="C56" s="29"/>
-      <c r="D56" s="29"/>
-      <c r="E56" s="29"/>
-      <c r="F56" s="29"/>
-      <c r="G56" s="29"/>
-      <c r="H56" s="29"/>
-    </row>
-    <row r="57" spans="1:8" s="30" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A57" s="29"/>
-      <c r="B57" s="29"/>
-      <c r="C57" s="29"/>
-      <c r="D57" s="29"/>
-      <c r="E57" s="29"/>
-      <c r="F57" s="29"/>
-      <c r="G57" s="29"/>
-      <c r="H57" s="29"/>
-    </row>
-    <row r="58" spans="1:8" s="30" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A58" s="29"/>
-      <c r="B58" s="29"/>
-      <c r="C58" s="29"/>
-      <c r="D58" s="29"/>
-      <c r="E58" s="29"/>
-      <c r="F58" s="29"/>
-      <c r="G58" s="29"/>
-      <c r="H58" s="29"/>
-    </row>
-    <row r="59" spans="1:8" s="30" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A59" s="29"/>
-      <c r="B59" s="29"/>
-      <c r="C59" s="29"/>
-      <c r="D59" s="29"/>
-      <c r="E59" s="29"/>
-      <c r="F59" s="29"/>
-      <c r="G59" s="29"/>
-      <c r="H59" s="29"/>
-    </row>
-    <row r="60" spans="1:8" s="30" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A60" s="29"/>
-      <c r="B60" s="29"/>
-      <c r="C60" s="29"/>
-      <c r="D60" s="29"/>
-      <c r="E60" s="29"/>
-      <c r="F60" s="29"/>
-      <c r="G60" s="29"/>
-      <c r="H60" s="29"/>
-    </row>
-    <row r="61" spans="1:8" s="30" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A61" s="29"/>
-      <c r="B61" s="29"/>
-      <c r="C61" s="29"/>
-      <c r="D61" s="29"/>
-      <c r="E61" s="29"/>
-      <c r="F61" s="29"/>
-      <c r="G61" s="29"/>
-      <c r="H61" s="29"/>
-    </row>
-    <row r="62" spans="1:8" s="30" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A62" s="29"/>
-      <c r="B62" s="29"/>
-      <c r="C62" s="29"/>
-      <c r="D62" s="29"/>
-      <c r="E62" s="29"/>
-      <c r="F62" s="29"/>
-      <c r="G62" s="29"/>
-      <c r="H62" s="29"/>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A63" s="8"/>
-      <c r="B63" s="9"/>
-      <c r="C63" s="9"/>
-      <c r="D63" s="9"/>
-      <c r="E63" s="10"/>
-      <c r="F63" s="9"/>
-      <c r="G63" s="9"/>
-      <c r="H63" s="9"/>
-    </row>
-    <row r="65" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A65" s="16" t="s">
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+    </row>
+    <row r="16" spans="1:8" s="16" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" s="15"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
+    </row>
+    <row r="17" spans="1:8" s="16" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" s="15"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
+    </row>
+    <row r="18" spans="1:8" s="16" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" s="15"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
+    </row>
+    <row r="19" spans="1:8" s="16" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" s="15"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
+    </row>
+    <row r="20" spans="1:8" s="16" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20" s="15"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15"/>
+    </row>
+    <row r="21" spans="1:8" s="16" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A21" s="15"/>
+      <c r="B21" s="15"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="15"/>
+    </row>
+    <row r="22" spans="1:8" s="16" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A22" s="15"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15"/>
+    </row>
+    <row r="23" spans="1:8" s="16" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A23" s="15"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="15"/>
+    </row>
+    <row r="24" spans="1:8" s="16" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A24" s="15"/>
+      <c r="B24" s="15"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="15"/>
+      <c r="H24" s="15"/>
+    </row>
+    <row r="25" spans="1:8" s="16" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A25" s="15"/>
+      <c r="B25" s="15"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="15"/>
+      <c r="H25" s="15"/>
+    </row>
+    <row r="26" spans="1:8" s="16" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A26" s="15"/>
+      <c r="B26" s="15"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="15"/>
+      <c r="G26" s="15"/>
+      <c r="H26" s="15"/>
+    </row>
+    <row r="27" spans="1:8" s="16" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A27" s="15"/>
+      <c r="B27" s="15"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="15"/>
+      <c r="H27" s="15"/>
+    </row>
+    <row r="28" spans="1:8" s="16" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A28" s="15"/>
+      <c r="B28" s="15"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="15"/>
+      <c r="F28" s="15"/>
+      <c r="G28" s="15"/>
+      <c r="H28" s="15"/>
+    </row>
+    <row r="29" spans="1:8" s="16" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A29" s="15"/>
+      <c r="B29" s="15"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="15"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="15"/>
+      <c r="G29" s="15"/>
+      <c r="H29" s="15"/>
+    </row>
+    <row r="30" spans="1:8" s="16" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A30" s="15"/>
+      <c r="B30" s="15"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="15"/>
+      <c r="F30" s="15"/>
+      <c r="G30" s="15"/>
+      <c r="H30" s="15"/>
+    </row>
+    <row r="31" spans="1:8" s="16" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A31" s="15"/>
+      <c r="B31" s="15"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="15"/>
+      <c r="F31" s="15"/>
+      <c r="G31" s="15"/>
+      <c r="H31" s="15"/>
+    </row>
+    <row r="32" spans="1:8" s="16" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A32" s="15"/>
+      <c r="B32" s="15"/>
+      <c r="C32" s="15"/>
+      <c r="D32" s="15"/>
+      <c r="E32" s="15"/>
+      <c r="F32" s="15"/>
+      <c r="G32" s="15"/>
+      <c r="H32" s="15"/>
+    </row>
+    <row r="33" spans="1:8" s="16" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A33" s="15"/>
+      <c r="B33" s="15"/>
+      <c r="C33" s="15"/>
+      <c r="D33" s="15"/>
+      <c r="E33" s="15"/>
+      <c r="F33" s="15"/>
+      <c r="G33" s="15"/>
+      <c r="H33" s="15"/>
+    </row>
+    <row r="34" spans="1:8" s="16" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A34" s="15"/>
+      <c r="B34" s="15"/>
+      <c r="C34" s="15"/>
+      <c r="D34" s="15"/>
+      <c r="E34" s="15"/>
+      <c r="F34" s="15"/>
+      <c r="G34" s="15"/>
+      <c r="H34" s="15"/>
+    </row>
+    <row r="35" spans="1:8" s="16" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A35" s="15"/>
+      <c r="B35" s="15"/>
+      <c r="C35" s="15"/>
+      <c r="D35" s="15"/>
+      <c r="E35" s="15"/>
+      <c r="F35" s="15"/>
+      <c r="G35" s="15"/>
+      <c r="H35" s="15"/>
+    </row>
+    <row r="36" spans="1:8" s="16" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A36" s="15"/>
+      <c r="B36" s="15"/>
+      <c r="C36" s="15"/>
+      <c r="D36" s="15"/>
+      <c r="E36" s="15"/>
+      <c r="F36" s="15"/>
+      <c r="G36" s="15"/>
+      <c r="H36" s="15"/>
+    </row>
+    <row r="37" spans="1:8" s="16" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A37" s="15"/>
+      <c r="B37" s="15"/>
+      <c r="C37" s="15"/>
+      <c r="D37" s="15"/>
+      <c r="E37" s="15"/>
+      <c r="F37" s="15"/>
+      <c r="G37" s="15"/>
+      <c r="H37" s="15"/>
+    </row>
+    <row r="38" spans="1:8" s="16" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A38" s="15"/>
+      <c r="B38" s="15"/>
+      <c r="C38" s="15"/>
+      <c r="D38" s="15"/>
+      <c r="E38" s="15"/>
+      <c r="F38" s="15"/>
+      <c r="G38" s="15"/>
+      <c r="H38" s="15"/>
+    </row>
+    <row r="39" spans="1:8" s="16" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A39" s="15"/>
+      <c r="B39" s="15"/>
+      <c r="C39" s="15"/>
+      <c r="D39" s="15"/>
+      <c r="E39" s="15"/>
+      <c r="F39" s="15"/>
+      <c r="G39" s="15"/>
+      <c r="H39" s="15"/>
+    </row>
+    <row r="40" spans="1:8" s="16" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A40" s="15"/>
+      <c r="B40" s="15"/>
+      <c r="C40" s="15"/>
+      <c r="D40" s="15"/>
+      <c r="E40" s="15"/>
+      <c r="F40" s="15"/>
+      <c r="G40" s="15"/>
+      <c r="H40" s="15"/>
+    </row>
+    <row r="41" spans="1:8" s="16" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A41" s="15"/>
+      <c r="B41" s="15"/>
+      <c r="C41" s="15"/>
+      <c r="D41" s="15"/>
+      <c r="E41" s="15"/>
+      <c r="F41" s="15"/>
+      <c r="G41" s="15"/>
+      <c r="H41" s="15"/>
+    </row>
+    <row r="42" spans="1:8" s="16" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A42" s="15"/>
+      <c r="B42" s="15"/>
+      <c r="C42" s="15"/>
+      <c r="D42" s="15"/>
+      <c r="E42" s="15"/>
+      <c r="F42" s="15"/>
+      <c r="G42" s="15"/>
+      <c r="H42" s="15"/>
+    </row>
+    <row r="43" spans="1:8" s="16" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A43" s="15"/>
+      <c r="B43" s="15"/>
+      <c r="C43" s="15"/>
+      <c r="D43" s="15"/>
+      <c r="E43" s="15"/>
+      <c r="F43" s="15"/>
+      <c r="G43" s="15"/>
+      <c r="H43" s="15"/>
+    </row>
+    <row r="44" spans="1:8" s="16" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A44" s="15"/>
+      <c r="B44" s="15"/>
+      <c r="C44" s="15"/>
+      <c r="D44" s="15"/>
+      <c r="E44" s="15"/>
+      <c r="F44" s="15"/>
+      <c r="G44" s="15"/>
+      <c r="H44" s="15"/>
+    </row>
+    <row r="45" spans="1:8" s="16" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A45" s="15"/>
+      <c r="B45" s="15"/>
+      <c r="C45" s="15"/>
+      <c r="D45" s="15"/>
+      <c r="E45" s="15"/>
+      <c r="F45" s="15"/>
+      <c r="G45" s="15"/>
+      <c r="H45" s="15"/>
+    </row>
+    <row r="46" spans="1:8" s="16" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A46" s="15"/>
+      <c r="B46" s="15"/>
+      <c r="C46" s="15"/>
+      <c r="D46" s="15"/>
+      <c r="E46" s="15"/>
+      <c r="F46" s="15"/>
+      <c r="G46" s="15"/>
+      <c r="H46" s="15"/>
+    </row>
+    <row r="47" spans="1:8" s="16" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A47" s="15"/>
+      <c r="B47" s="15"/>
+      <c r="C47" s="15"/>
+      <c r="D47" s="15"/>
+      <c r="E47" s="15"/>
+      <c r="F47" s="15"/>
+      <c r="G47" s="15"/>
+      <c r="H47" s="15"/>
+    </row>
+    <row r="48" spans="1:8" s="16" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A48" s="15"/>
+      <c r="B48" s="15"/>
+      <c r="C48" s="15"/>
+      <c r="D48" s="15"/>
+      <c r="E48" s="15"/>
+      <c r="F48" s="15"/>
+      <c r="G48" s="15"/>
+      <c r="H48" s="15"/>
+    </row>
+    <row r="49" spans="1:8" s="16" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A49" s="15"/>
+      <c r="B49" s="15"/>
+      <c r="C49" s="15"/>
+      <c r="D49" s="15"/>
+      <c r="E49" s="15"/>
+      <c r="F49" s="15"/>
+      <c r="G49" s="15"/>
+      <c r="H49" s="15"/>
+    </row>
+    <row r="50" spans="1:8" s="16" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A50" s="15"/>
+      <c r="B50" s="15"/>
+      <c r="C50" s="15"/>
+      <c r="D50" s="15"/>
+      <c r="E50" s="15"/>
+      <c r="F50" s="15"/>
+      <c r="G50" s="15"/>
+      <c r="H50" s="15"/>
+    </row>
+    <row r="51" spans="1:8" s="16" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A51" s="15"/>
+      <c r="B51" s="15"/>
+      <c r="C51" s="15"/>
+      <c r="D51" s="15"/>
+      <c r="E51" s="15"/>
+      <c r="F51" s="15"/>
+      <c r="G51" s="15"/>
+      <c r="H51" s="15"/>
+    </row>
+    <row r="52" spans="1:8" s="16" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A52" s="15"/>
+      <c r="B52" s="15"/>
+      <c r="C52" s="15"/>
+      <c r="D52" s="15"/>
+      <c r="E52" s="15"/>
+      <c r="F52" s="15"/>
+      <c r="G52" s="15"/>
+      <c r="H52" s="15"/>
+    </row>
+    <row r="53" spans="1:8" s="16" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A53" s="15"/>
+      <c r="B53" s="15"/>
+      <c r="C53" s="15"/>
+      <c r="D53" s="15"/>
+      <c r="E53" s="15"/>
+      <c r="F53" s="15"/>
+      <c r="G53" s="15"/>
+      <c r="H53" s="15"/>
+    </row>
+    <row r="54" spans="1:8" s="16" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A54" s="15"/>
+      <c r="B54" s="15"/>
+      <c r="C54" s="15"/>
+      <c r="D54" s="15"/>
+      <c r="E54" s="15"/>
+      <c r="F54" s="15"/>
+      <c r="G54" s="15"/>
+      <c r="H54" s="15"/>
+    </row>
+    <row r="55" spans="1:8" s="16" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A55" s="15"/>
+      <c r="B55" s="15"/>
+      <c r="C55" s="15"/>
+      <c r="D55" s="15"/>
+      <c r="E55" s="15"/>
+      <c r="F55" s="15"/>
+      <c r="G55" s="15"/>
+      <c r="H55" s="15"/>
+    </row>
+    <row r="56" spans="1:8" s="16" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A56" s="15"/>
+      <c r="B56" s="15"/>
+      <c r="C56" s="15"/>
+      <c r="D56" s="15"/>
+      <c r="E56" s="15"/>
+      <c r="F56" s="15"/>
+      <c r="G56" s="15"/>
+      <c r="H56" s="15"/>
+    </row>
+    <row r="57" spans="1:8" s="16" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A57" s="15"/>
+      <c r="B57" s="15"/>
+      <c r="C57" s="15"/>
+      <c r="D57" s="15"/>
+      <c r="E57" s="15"/>
+      <c r="F57" s="15"/>
+      <c r="G57" s="15"/>
+      <c r="H57" s="15"/>
+    </row>
+    <row r="58" spans="1:8" s="16" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A58" s="15"/>
+      <c r="B58" s="15"/>
+      <c r="C58" s="15"/>
+      <c r="D58" s="15"/>
+      <c r="E58" s="15"/>
+      <c r="F58" s="15"/>
+      <c r="G58" s="15"/>
+      <c r="H58" s="15"/>
+    </row>
+    <row r="59" spans="1:8" s="16" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A59" s="15"/>
+      <c r="B59" s="15"/>
+      <c r="C59" s="15"/>
+      <c r="D59" s="15"/>
+      <c r="E59" s="15"/>
+      <c r="F59" s="15"/>
+      <c r="G59" s="15"/>
+      <c r="H59" s="15"/>
+    </row>
+    <row r="60" spans="1:8" s="16" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A60" s="15"/>
+      <c r="B60" s="15"/>
+      <c r="C60" s="15"/>
+      <c r="D60" s="15"/>
+      <c r="E60" s="15"/>
+      <c r="F60" s="15"/>
+      <c r="G60" s="15"/>
+      <c r="H60" s="15"/>
+    </row>
+    <row r="61" spans="1:8" s="16" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A61" s="15"/>
+      <c r="B61" s="15"/>
+      <c r="C61" s="15"/>
+      <c r="D61" s="15"/>
+      <c r="E61" s="15"/>
+      <c r="F61" s="15"/>
+      <c r="G61" s="15"/>
+      <c r="H61" s="15"/>
+    </row>
+    <row r="62" spans="1:8" s="16" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A62" s="15"/>
+      <c r="B62" s="15"/>
+      <c r="C62" s="15"/>
+      <c r="D62" s="15"/>
+      <c r="E62" s="15"/>
+      <c r="F62" s="15"/>
+      <c r="G62" s="15"/>
+      <c r="H62" s="15"/>
+    </row>
+    <row r="63" spans="1:8" s="16" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A63" s="15"/>
+      <c r="B63" s="15"/>
+      <c r="C63" s="15"/>
+      <c r="D63" s="15"/>
+      <c r="E63" s="15"/>
+      <c r="F63" s="15"/>
+      <c r="G63" s="15"/>
+      <c r="H63" s="15"/>
+    </row>
+    <row r="64" spans="1:8" s="16" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A64" s="15"/>
+      <c r="B64" s="15"/>
+      <c r="C64" s="15"/>
+      <c r="D64" s="15"/>
+      <c r="E64" s="15"/>
+      <c r="F64" s="15"/>
+      <c r="G64" s="15"/>
+      <c r="H64" s="15"/>
+    </row>
+    <row r="65" spans="1:8" s="16" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A65" s="15"/>
+      <c r="B65" s="15"/>
+      <c r="C65" s="15"/>
+      <c r="D65" s="15"/>
+      <c r="E65" s="15"/>
+      <c r="F65" s="15"/>
+      <c r="G65" s="15"/>
+      <c r="H65" s="15"/>
+    </row>
+    <row r="66" spans="1:8" s="16" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A66" s="15"/>
+      <c r="B66" s="15"/>
+      <c r="C66" s="15"/>
+      <c r="D66" s="15"/>
+      <c r="E66" s="15"/>
+      <c r="F66" s="15"/>
+      <c r="G66" s="15"/>
+      <c r="H66" s="15"/>
+    </row>
+    <row r="67" spans="1:8" s="16" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A67" s="15"/>
+      <c r="B67" s="15"/>
+      <c r="C67" s="15"/>
+      <c r="D67" s="15"/>
+      <c r="E67" s="15"/>
+      <c r="F67" s="15"/>
+      <c r="G67" s="15"/>
+      <c r="H67" s="15"/>
+    </row>
+    <row r="68" spans="1:8" s="16" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A68" s="15"/>
+      <c r="B68" s="15"/>
+      <c r="C68" s="15"/>
+      <c r="D68" s="15"/>
+      <c r="E68" s="15"/>
+      <c r="F68" s="15"/>
+      <c r="G68" s="15"/>
+      <c r="H68" s="15"/>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A69" s="8"/>
+      <c r="B69" s="9"/>
+      <c r="C69" s="9"/>
+      <c r="D69" s="9"/>
+      <c r="E69" s="10"/>
+      <c r="F69" s="9"/>
+      <c r="G69" s="9"/>
+      <c r="H69" s="9"/>
+    </row>
+    <row r="71" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A71" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="B65" s="16"/>
-      <c r="C65" s="16"/>
-      <c r="D65" s="16"/>
-      <c r="E65" s="16"/>
-      <c r="F65" s="16"/>
-      <c r="G65" s="16"/>
-      <c r="H65" s="16"/>
-    </row>
-    <row r="66" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A66" s="22" t="s">
+      <c r="B71" s="21"/>
+      <c r="C71" s="21"/>
+      <c r="D71" s="21"/>
+      <c r="E71" s="21"/>
+      <c r="F71" s="21"/>
+      <c r="G71" s="21"/>
+      <c r="H71" s="21"/>
+    </row>
+    <row r="72" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A72" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="B66" s="25">
+      <c r="B72" s="30">
         <f>COUNTA(D:D)-6</f>
         <v>0</v>
       </c>
-      <c r="C66" s="1" t="s">
+      <c r="C72" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D66" s="2">
+      <c r="D72" s="2">
         <f>COUNTIF(E:E,"Pass")</f>
         <v>0</v>
       </c>
-      <c r="E66" s="1" t="s">
+      <c r="E72" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F66" s="19">
+      <c r="F72" s="24">
         <f>COUNTIF(E:E,"Fail")-1</f>
         <v>0</v>
       </c>
-      <c r="G66" s="20"/>
-      <c r="H66" s="21"/>
-    </row>
-    <row r="67" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A67" s="23"/>
-      <c r="B67" s="26"/>
-      <c r="C67" s="1" t="s">
+      <c r="G72" s="25"/>
+      <c r="H72" s="26"/>
+    </row>
+    <row r="73" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A73" s="28"/>
+      <c r="B73" s="31"/>
+      <c r="C73" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D67" s="2">
+      <c r="D73" s="2">
         <f>COUNTIF(E:E,"Partial Pass")</f>
         <v>0</v>
       </c>
-      <c r="E67" s="1" t="s">
+      <c r="E73" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F67" s="19">
+      <c r="F73" s="24">
         <f>COUNTIF(E:E,"Not Completed")-1</f>
         <v>0</v>
       </c>
-      <c r="G67" s="20"/>
-      <c r="H67" s="21"/>
-    </row>
-    <row r="68" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A68" s="24"/>
-      <c r="B68" s="27"/>
-      <c r="C68" s="1" t="s">
+      <c r="G73" s="25"/>
+      <c r="H73" s="26"/>
+    </row>
+    <row r="74" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A74" s="29"/>
+      <c r="B74" s="32"/>
+      <c r="C74" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D68" s="2">
+      <c r="D74" s="2">
         <f>COUNTIF(E:E,"Inapplicable")</f>
         <v>0</v>
       </c>
-      <c r="E68" s="3"/>
-      <c r="F68" s="19"/>
-      <c r="G68" s="20"/>
-      <c r="H68" s="21"/>
-    </row>
-    <row r="69" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A69" s="1" t="s">
+      <c r="E74" s="3"/>
+      <c r="F74" s="24"/>
+      <c r="G74" s="25"/>
+      <c r="H74" s="26"/>
+    </row>
+    <row r="75" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A75" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B69" s="14" t="s">
+      <c r="B75" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="C69" s="14"/>
-      <c r="D69" s="17" t="s">
+      <c r="C75" s="19"/>
+      <c r="D75" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="E69" s="18"/>
-      <c r="F69" s="14"/>
-      <c r="G69" s="14"/>
-      <c r="H69" s="14"/>
-    </row>
-    <row r="70" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A70" s="1" t="s">
+      <c r="E75" s="23"/>
+      <c r="F75" s="19"/>
+      <c r="G75" s="19"/>
+      <c r="H75" s="19"/>
+    </row>
+    <row r="76" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A76" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B70" s="15" t="s">
+      <c r="B76" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="C70" s="15"/>
-      <c r="D70" s="17" t="s">
+      <c r="C76" s="20"/>
+      <c r="D76" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="E70" s="18"/>
-      <c r="F70" s="15">
+      <c r="E76" s="23"/>
+      <c r="F76" s="20">
         <v>2</v>
       </c>
-      <c r="G70" s="15"/>
-      <c r="H70" s="14"/>
-    </row>
-    <row r="71" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A71" s="4" t="s">
+      <c r="G76" s="20"/>
+      <c r="H76" s="19"/>
+    </row>
+    <row r="77" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A77" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B71" s="15" t="s">
+      <c r="B77" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C71" s="14"/>
-      <c r="D71" s="14"/>
-      <c r="E71" s="14"/>
-      <c r="F71" s="14"/>
-      <c r="G71" s="14"/>
-      <c r="H71" s="14"/>
+      <c r="C77" s="19"/>
+      <c r="D77" s="19"/>
+      <c r="E77" s="19"/>
+      <c r="F77" s="19"/>
+      <c r="G77" s="19"/>
+      <c r="H77" s="19"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:H2"/>
   <mergeCells count="13">
-    <mergeCell ref="F69:H69"/>
-    <mergeCell ref="F70:H70"/>
-    <mergeCell ref="A65:H65"/>
-    <mergeCell ref="B71:H71"/>
-    <mergeCell ref="D69:E69"/>
-    <mergeCell ref="D70:E70"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="F66:H66"/>
-    <mergeCell ref="F67:H67"/>
-    <mergeCell ref="A66:A68"/>
-    <mergeCell ref="B66:B68"/>
-    <mergeCell ref="F68:H68"/>
+    <mergeCell ref="F75:H75"/>
+    <mergeCell ref="F76:H76"/>
+    <mergeCell ref="A71:H71"/>
+    <mergeCell ref="B77:H77"/>
+    <mergeCell ref="D75:E75"/>
+    <mergeCell ref="D76:E76"/>
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="B75:C75"/>
+    <mergeCell ref="F72:H72"/>
+    <mergeCell ref="F73:H73"/>
+    <mergeCell ref="A72:A74"/>
+    <mergeCell ref="B72:B74"/>
+    <mergeCell ref="F74:H74"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E69:E1048576 E64:E65">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E75:E1048576 E70:E71">
       <formula1>"通过,不通过,无法执行"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1">
@@ -2234,12 +2323,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
   <documentManagement/>
 </p:properties>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="文档" ma:contentTypeID="0x010100E4333E5FE2FE9646B7C5A1EFED3F06AD" ma:contentTypeVersion="0" ma:contentTypeDescription="新建文档。" ma:contentTypeScope="" ma:versionID="6c373dede930dc4ccd3742d43cfc23a5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b51e50da1bca0add1c6bbfbefcbaaafa">
     <xsd:element name="properties">
@@ -2288,16 +2386,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5321DAAF-CDE3-4627-AE30-FA281AB8C330}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B24E75A5-90DA-44AB-9E61-2AD833E918FA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
@@ -2311,7 +2408,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CDCD5941-9B82-44F5-97A1-AFDDB7A99BBB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2324,12 +2421,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5321DAAF-CDE3-4627-AE30-FA281AB8C330}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>